<commit_message>
Asignación de recursos en GRECO
Se han asignado a Jennifer y Cristhian los  recursos de matemáticas 8
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion03/Escaleta MA_07_03_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion03/Escaleta MA_07_03_CO.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Matematicas\fuentes\contenidos\grado07\guion03\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lzambrano\Documents\GitHub\Matematicas\fuentes\contenidos\grado07\guion03\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,12 +16,12 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" iterateCount="2" iterateDelta="10"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="349">
   <si>
     <t>Asignatura</t>
   </si>
@@ -1063,6 +1063,12 @@
   </si>
   <si>
     <t>Recurso M102AB-02</t>
+  </si>
+  <si>
+    <t>Andrea</t>
+  </si>
+  <si>
+    <t>Johanna</t>
   </si>
 </sst>
 </file>
@@ -1159,7 +1165,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1241,6 +1247,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1451,7 +1463,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1744,6 +1756,69 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1759,68 +1834,11 @@
     <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6414,8 +6432,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z183"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="V30" sqref="V30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -6456,65 +6474,65 @@
       <c r="R1" s="31"/>
     </row>
     <row r="2" spans="1:24" s="62" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="125" t="s">
+      <c r="A2" s="120" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="124" t="s">
+      <c r="B2" s="119" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="132" t="s">
+      <c r="C2" s="127" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="133" t="s">
+      <c r="D2" s="128" t="s">
         <v>296</v>
       </c>
-      <c r="E2" s="124" t="s">
+      <c r="E2" s="119" t="s">
         <v>297</v>
       </c>
-      <c r="F2" s="136" t="s">
+      <c r="F2" s="131" t="s">
         <v>298</v>
       </c>
-      <c r="G2" s="131" t="s">
+      <c r="G2" s="126" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="136" t="s">
+      <c r="H2" s="131" t="s">
         <v>299</v>
       </c>
-      <c r="I2" s="136" t="s">
+      <c r="I2" s="131" t="s">
         <v>300</v>
       </c>
-      <c r="J2" s="128" t="s">
+      <c r="J2" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="126" t="s">
+      <c r="K2" s="121" t="s">
         <v>301</v>
       </c>
       <c r="L2" s="110" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="130" t="s">
+      <c r="M2" s="125" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="130"/>
-      <c r="O2" s="123" t="s">
+      <c r="N2" s="125"/>
+      <c r="O2" s="118" t="s">
         <v>199</v>
       </c>
-      <c r="P2" s="112" t="s">
+      <c r="P2" s="133" t="s">
         <v>302</v>
       </c>
-      <c r="Q2" s="114" t="s">
+      <c r="Q2" s="135" t="s">
         <v>121</v>
       </c>
-      <c r="R2" s="116" t="s">
+      <c r="R2" s="137" t="s">
         <v>122</v>
       </c>
-      <c r="S2" s="114" t="s">
+      <c r="S2" s="135" t="s">
         <v>123</v>
       </c>
-      <c r="T2" s="115" t="s">
+      <c r="T2" s="136" t="s">
         <v>124</v>
       </c>
-      <c r="U2" s="114" t="s">
+      <c r="U2" s="135" t="s">
         <v>125</v>
       </c>
       <c r="X2" s="110" t="s">
@@ -6522,17 +6540,17 @@
       </c>
     </row>
     <row r="3" spans="1:24" s="62" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="125"/>
-      <c r="B3" s="124"/>
-      <c r="C3" s="132"/>
-      <c r="D3" s="134"/>
-      <c r="E3" s="135"/>
-      <c r="F3" s="137"/>
-      <c r="G3" s="131"/>
-      <c r="H3" s="137"/>
-      <c r="I3" s="137"/>
-      <c r="J3" s="129"/>
-      <c r="K3" s="127"/>
+      <c r="A3" s="120"/>
+      <c r="B3" s="119"/>
+      <c r="C3" s="127"/>
+      <c r="D3" s="129"/>
+      <c r="E3" s="130"/>
+      <c r="F3" s="132"/>
+      <c r="G3" s="126"/>
+      <c r="H3" s="132"/>
+      <c r="I3" s="132"/>
+      <c r="J3" s="124"/>
+      <c r="K3" s="122"/>
       <c r="L3" s="111"/>
       <c r="M3" s="59" t="s">
         <v>126</v>
@@ -6540,13 +6558,13 @@
       <c r="N3" s="59" t="s">
         <v>127</v>
       </c>
-      <c r="O3" s="123"/>
-      <c r="P3" s="113"/>
-      <c r="Q3" s="114"/>
-      <c r="R3" s="116"/>
-      <c r="S3" s="114"/>
-      <c r="T3" s="115"/>
-      <c r="U3" s="114"/>
+      <c r="O3" s="118"/>
+      <c r="P3" s="134"/>
+      <c r="Q3" s="135"/>
+      <c r="R3" s="137"/>
+      <c r="S3" s="135"/>
+      <c r="T3" s="136"/>
+      <c r="U3" s="135"/>
       <c r="X3" s="111"/>
     </row>
     <row r="4" spans="1:24" s="67" customFormat="1" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -6607,6 +6625,9 @@
       <c r="U4" s="100" t="s">
         <v>212</v>
       </c>
+      <c r="V4" s="138" t="s">
+        <v>347</v>
+      </c>
       <c r="X4" s="34" t="s">
         <v>202</v>
       </c>
@@ -6669,6 +6690,9 @@
       <c r="U5" s="103" t="s">
         <v>216</v>
       </c>
+      <c r="V5" s="138" t="s">
+        <v>347</v>
+      </c>
       <c r="X5" s="34" t="s">
         <v>202</v>
       </c>
@@ -6733,6 +6757,9 @@
       <c r="U6" s="103" t="s">
         <v>212</v>
       </c>
+      <c r="V6" s="139" t="s">
+        <v>348</v>
+      </c>
       <c r="X6" s="34" t="s">
         <v>201</v>
       </c>
@@ -6797,6 +6824,9 @@
       <c r="U7" s="103" t="s">
         <v>216</v>
       </c>
+      <c r="V7" s="139" t="s">
+        <v>348</v>
+      </c>
       <c r="X7" s="38" t="s">
         <v>204</v>
       </c>
@@ -6861,6 +6891,9 @@
       <c r="U8" s="103" t="s">
         <v>216</v>
       </c>
+      <c r="V8" s="139" t="s">
+        <v>348</v>
+      </c>
       <c r="X8" s="38" t="s">
         <v>203</v>
       </c>
@@ -6925,6 +6958,9 @@
       <c r="U9" s="103" t="s">
         <v>212</v>
       </c>
+      <c r="V9" s="139" t="s">
+        <v>348</v>
+      </c>
       <c r="X9" s="38" t="s">
         <v>201</v>
       </c>
@@ -6989,6 +7025,9 @@
       <c r="U10" s="103" t="s">
         <v>216</v>
       </c>
+      <c r="V10" s="139" t="s">
+        <v>348</v>
+      </c>
       <c r="X10" s="38" t="s">
         <v>201</v>
       </c>
@@ -7053,6 +7092,9 @@
       <c r="U11" s="103" t="s">
         <v>216</v>
       </c>
+      <c r="V11" s="139" t="s">
+        <v>348</v>
+      </c>
       <c r="X11" s="38" t="s">
         <v>204</v>
       </c>
@@ -7117,6 +7159,9 @@
       <c r="U12" s="103" t="s">
         <v>216</v>
       </c>
+      <c r="V12" s="139" t="s">
+        <v>348</v>
+      </c>
       <c r="X12" s="38" t="s">
         <v>201</v>
       </c>
@@ -7181,6 +7226,9 @@
       <c r="U13" s="103" t="s">
         <v>216</v>
       </c>
+      <c r="V13" s="138" t="s">
+        <v>347</v>
+      </c>
       <c r="X13" s="38" t="s">
         <v>202</v>
       </c>
@@ -7245,6 +7293,9 @@
       <c r="U14" s="103" t="s">
         <v>216</v>
       </c>
+      <c r="V14" s="138" t="s">
+        <v>347</v>
+      </c>
       <c r="X14" s="38" t="s">
         <v>203</v>
       </c>
@@ -7306,6 +7357,9 @@
       </c>
       <c r="U15" s="106" t="s">
         <v>343</v>
+      </c>
+      <c r="V15" s="138" t="s">
+        <v>347</v>
       </c>
       <c r="X15" s="38" t="s">
         <v>204</v>
@@ -7369,6 +7423,9 @@
       <c r="U16" s="103" t="s">
         <v>212</v>
       </c>
+      <c r="V16" s="138" t="s">
+        <v>347</v>
+      </c>
       <c r="X16" s="38" t="s">
         <v>201</v>
       </c>
@@ -7431,6 +7488,9 @@
       <c r="U17" s="103" t="s">
         <v>216</v>
       </c>
+      <c r="V17" s="138" t="s">
+        <v>347</v>
+      </c>
       <c r="X17" s="38" t="s">
         <v>205</v>
       </c>
@@ -7491,6 +7551,9 @@
       <c r="U18" s="103" t="s">
         <v>216</v>
       </c>
+      <c r="V18" s="138" t="s">
+        <v>347</v>
+      </c>
       <c r="X18" s="38" t="s">
         <v>204</v>
       </c>
@@ -7553,6 +7616,9 @@
       <c r="U19" s="103" t="s">
         <v>216</v>
       </c>
+      <c r="V19" s="138" t="s">
+        <v>347</v>
+      </c>
       <c r="X19" s="38" t="s">
         <v>202</v>
       </c>
@@ -7615,6 +7681,9 @@
       <c r="U20" s="103" t="s">
         <v>216</v>
       </c>
+      <c r="V20" s="138" t="s">
+        <v>347</v>
+      </c>
       <c r="X20" s="38" t="s">
         <v>203</v>
       </c>
@@ -7679,6 +7748,9 @@
       <c r="U21" s="103" t="s">
         <v>212</v>
       </c>
+      <c r="V21" s="139" t="s">
+        <v>348</v>
+      </c>
       <c r="X21" s="38" t="s">
         <v>201</v>
       </c>
@@ -7743,6 +7815,9 @@
       <c r="U22" s="103" t="s">
         <v>216</v>
       </c>
+      <c r="V22" s="138" t="s">
+        <v>347</v>
+      </c>
       <c r="X22" s="38" t="s">
         <v>202</v>
       </c>
@@ -7807,6 +7882,9 @@
       <c r="U23" s="103" t="s">
         <v>216</v>
       </c>
+      <c r="V23" s="138" t="s">
+        <v>347</v>
+      </c>
       <c r="X23" s="38" t="s">
         <v>204</v>
       </c>
@@ -7870,6 +7948,9 @@
       </c>
       <c r="U24" s="103" t="s">
         <v>216</v>
+      </c>
+      <c r="V24" s="138" t="s">
+        <v>347</v>
       </c>
       <c r="X24" s="38" t="s">
         <v>203</v>
@@ -7933,6 +8014,9 @@
       <c r="U25" s="103" t="s">
         <v>212</v>
       </c>
+      <c r="V25" s="139" t="s">
+        <v>348</v>
+      </c>
       <c r="X25" s="38" t="s">
         <v>205</v>
       </c>
@@ -7995,6 +8079,9 @@
       <c r="U26" s="103" t="s">
         <v>216</v>
       </c>
+      <c r="V26" s="139" t="s">
+        <v>348</v>
+      </c>
       <c r="X26" s="38" t="s">
         <v>204</v>
       </c>
@@ -8058,6 +8145,9 @@
       </c>
       <c r="U27" s="103" t="s">
         <v>216</v>
+      </c>
+      <c r="V27" s="139" t="s">
+        <v>348</v>
       </c>
       <c r="X27" s="38" t="s">
         <v>203</v>
@@ -8121,6 +8211,9 @@
       <c r="U28" s="103" t="s">
         <v>216</v>
       </c>
+      <c r="V28" s="139" t="s">
+        <v>348</v>
+      </c>
       <c r="X28" s="38" t="s">
         <v>205</v>
       </c>
@@ -8183,6 +8276,9 @@
       <c r="U29" s="103" t="s">
         <v>212</v>
       </c>
+      <c r="V29" s="138" t="s">
+        <v>347</v>
+      </c>
       <c r="X29" s="38" t="s">
         <v>203</v>
       </c>
@@ -8244,6 +8340,9 @@
       </c>
       <c r="U30" s="106" t="s">
         <v>216</v>
+      </c>
+      <c r="V30" s="138" t="s">
+        <v>347</v>
       </c>
       <c r="X30" s="38" t="s">
         <v>203</v>
@@ -8347,6 +8446,9 @@
       <c r="U32" s="103" t="s">
         <v>216</v>
       </c>
+      <c r="V32" s="138" t="s">
+        <v>347</v>
+      </c>
       <c r="X32" s="38" t="s">
         <v>205</v>
       </c>
@@ -8386,6 +8488,9 @@
       </c>
       <c r="U33" s="103" t="s">
         <v>216</v>
+      </c>
+      <c r="V33" s="138" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="34" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -8461,33 +8566,33 @@
       <c r="Z36" s="31"/>
     </row>
     <row r="37" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="117" t="s">
+      <c r="A37" s="112" t="s">
         <v>240</v>
       </c>
-      <c r="B37" s="118"/>
-      <c r="C37" s="118"/>
-      <c r="D37" s="118"/>
-      <c r="E37" s="118"/>
-      <c r="F37" s="118"/>
-      <c r="G37" s="118"/>
-      <c r="H37" s="118"/>
-      <c r="I37" s="118"/>
-      <c r="J37" s="118"/>
-      <c r="K37" s="119"/>
+      <c r="B37" s="113"/>
+      <c r="C37" s="113"/>
+      <c r="D37" s="113"/>
+      <c r="E37" s="113"/>
+      <c r="F37" s="113"/>
+      <c r="G37" s="113"/>
+      <c r="H37" s="113"/>
+      <c r="I37" s="113"/>
+      <c r="J37" s="113"/>
+      <c r="K37" s="114"/>
       <c r="Z37" s="31"/>
     </row>
     <row r="38" spans="1:26" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="120"/>
-      <c r="B38" s="121"/>
-      <c r="C38" s="121"/>
-      <c r="D38" s="121"/>
-      <c r="E38" s="121"/>
-      <c r="F38" s="121"/>
-      <c r="G38" s="121"/>
-      <c r="H38" s="121"/>
-      <c r="I38" s="121"/>
-      <c r="J38" s="121"/>
-      <c r="K38" s="122"/>
+      <c r="A38" s="115"/>
+      <c r="B38" s="116"/>
+      <c r="C38" s="116"/>
+      <c r="D38" s="116"/>
+      <c r="E38" s="116"/>
+      <c r="F38" s="116"/>
+      <c r="G38" s="116"/>
+      <c r="H38" s="116"/>
+      <c r="I38" s="116"/>
+      <c r="J38" s="116"/>
+      <c r="K38" s="117"/>
       <c r="Z38" s="31"/>
     </row>
     <row r="39" spans="1:26" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -9551,6 +9656,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="P2:P3"/>
+    <mergeCell ref="U2:U3"/>
+    <mergeCell ref="T2:T3"/>
+    <mergeCell ref="S2:S3"/>
+    <mergeCell ref="R2:R3"/>
+    <mergeCell ref="Q2:Q3"/>
     <mergeCell ref="X2:X3"/>
     <mergeCell ref="A37:K38"/>
     <mergeCell ref="O2:O3"/>
@@ -9567,15 +9678,9 @@
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="L2:L3"/>
-    <mergeCell ref="P2:P3"/>
-    <mergeCell ref="U2:U3"/>
-    <mergeCell ref="T2:T3"/>
-    <mergeCell ref="S2:S3"/>
-    <mergeCell ref="R2:R3"/>
-    <mergeCell ref="Q2:Q3"/>
   </mergeCells>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="V20 P4:P5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P4:P5">
       <formula1>$W$22:$W$23</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="X4:X32">

</xml_diff>